<commit_message>
Introduced new parts that can be purchased for manufacturing by NextPCB. Corrected numerous issues.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,24 +5,24 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Courses/KiCad/KLP 5e ESP32 sensor board/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/T7/Kicad/KLP 5e ESP32 sensor board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0479D957-6838-8B40-A196-DDD9EAEE42CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5710E97F-3BB4-7540-B3AB-367B3E0EFFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38900" yWindow="-480" windowWidth="38400" windowHeight="21100" xr2:uid="{07068760-EA20-DB4D-BBEF-E64F73D6D957}"/>
+    <workbookView xWindow="41440" yWindow="-620" windowWidth="38400" windowHeight="21100" xr2:uid="{07068760-EA20-DB4D-BBEF-E64F73D6D957}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="152">
   <si>
     <t>DESIGNATOR</t>
   </si>
@@ -162,9 +162,6 @@
     <t>USB_C_Receptacle</t>
   </si>
   <si>
-    <t>USB 2.0-only Type-C Receptacle connector</t>
-  </si>
-  <si>
     <t xml:space="preserve">    J2</t>
   </si>
   <si>
@@ -330,9 +327,6 @@
     <t>1101NE</t>
   </si>
   <si>
-    <t>SMD_6x3.5mm_h2.5mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">    U1</t>
   </si>
   <si>
@@ -357,18 +351,6 @@
     <t>LM1117MPX-3.3_NOPB</t>
   </si>
   <si>
-    <t>LM1117MPX-3.3/NOPB</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>SOT-223-4</t>
-  </si>
-  <si>
-    <t>Space saving 800-mA low-dropout linear regulator with internal current limit</t>
-  </si>
-  <si>
     <t xml:space="preserve">    U3</t>
   </si>
   <si>
@@ -459,13 +441,43 @@
     <t>Belfuse</t>
   </si>
   <si>
-    <t>Valcon</t>
-  </si>
-  <si>
-    <t>CONN-14122</t>
-  </si>
-  <si>
     <t>JST_B2B-PH-SM4-TB</t>
+  </si>
+  <si>
+    <t>Footprints:BELFUSE_SS-52400-002</t>
+  </si>
+  <si>
+    <t>LM1117MPX-33NOPB</t>
+  </si>
+  <si>
+    <t>On Semiconductor</t>
+  </si>
+  <si>
+    <t>SOT−223 CASE 318H</t>
+  </si>
+  <si>
+    <t>See https://www.snapeda.com/parts/LM1117MPX-33NOPB/ON%20Semiconductor/view-part/?welcome=home&amp;ref=search&amp;t=LM1117MPX-3.3_NOPB</t>
+  </si>
+  <si>
+    <t>USLPT2819 MSLPT (Mini size)</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>USLPT2819 Family</t>
+  </si>
+  <si>
+    <t>SMD_6x3.5mm_h2.5mm. Please see https://www.snapeda.com/parts/USLPT2819DT2TR/TE%20Connectivity/view-part/?ref=search&amp;t=SMD%20switch</t>
+  </si>
+  <si>
+    <t>USB 2.0-only Type-C Receptacle connector. See https://www.snapeda.com/parts/SS-52400-002/Bel%20Fuse/view-part/?ref=search&amp;t=BELFUSE_SS-52400-002</t>
+  </si>
+  <si>
+    <t>BELFUSE Stewart Connector</t>
+  </si>
+  <si>
+    <t>SS-52400-003 for standard 1.6 mm PCB thickness</t>
   </si>
 </sst>
 </file>
@@ -507,12 +519,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -535,9 +553,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1" xr:uid="{3B013FD0-0971-5A4F-BE89-C1629EA6565E}"/>
@@ -879,13 +898,14 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="3" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="54.5703125" customWidth="1"/>
@@ -1112,7 +1132,7 @@
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F10">
         <v>1210</v>
@@ -1122,233 +1142,236 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D11" t="s">
-        <v>146</v>
-      </c>
-      <c r="E11" t="s">
-        <v>145</v>
-      </c>
-      <c r="G11" t="s">
-        <v>46</v>
+      <c r="D11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
         <v>47</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" t="s">
         <v>48</v>
       </c>
-      <c r="D12" t="s">
-        <v>147</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>49</v>
-      </c>
-      <c r="G12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>51</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>53</v>
-      </c>
-      <c r="G13" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" t="s">
         <v>57</v>
-      </c>
-      <c r="E14" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>59</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="G15" t="s">
         <v>60</v>
-      </c>
-      <c r="G15" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
         <v>62</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" t="s">
         <v>63</v>
       </c>
-      <c r="D16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>64</v>
-      </c>
-      <c r="G16" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
         <v>66</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s">
         <v>67</v>
       </c>
-      <c r="D17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>68</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>69</v>
-      </c>
-      <c r="G17" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
         <v>72</v>
       </c>
-      <c r="D18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>73</v>
-      </c>
-      <c r="G18" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F19">
         <v>805</v>
       </c>
       <c r="G19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" t="s">
         <v>79</v>
       </c>
-      <c r="F20" t="s">
-        <v>80</v>
-      </c>
       <c r="G20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
         <v>83</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>84</v>
-      </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -1357,15 +1380,15 @@
         <v>470</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1374,66 +1397,66 @@
         <v>330</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>88</v>
-      </c>
       <c r="F25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
         <v>89</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>90</v>
-      </c>
       <c r="F26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
         <v>91</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>92</v>
-      </c>
       <c r="F27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -1442,259 +1465,265 @@
         <v>50</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
         <v>98</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="F31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F31" t="s">
-        <v>80</v>
-      </c>
-      <c r="G31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B32" s="2">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" t="s">
-        <v>102</v>
+      <c r="D32" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" t="s">
         <v>103</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>104</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" t="s">
         <v>105</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>106</v>
       </c>
-      <c r="F33" t="s">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G33" t="s">
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E34" t="s">
-        <v>112</v>
-      </c>
-      <c r="F34" t="s">
-        <v>113</v>
-      </c>
-      <c r="G34" t="s">
-        <v>114</v>
+      <c r="D34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D36" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E36" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F36" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G36" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D37" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E37" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F37" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G37" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D38" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E38" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F38" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G38" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E39" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F39" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G39" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D40" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E40" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F40" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G40" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated U1 footprint to better match the component we can order from Microchip.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/T7/Kicad/KLP 5e ESP32 sensor board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5710E97F-3BB4-7540-B3AB-367B3E0EFFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F193C40E-F788-5742-BEF8-D4646FCDD4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41440" yWindow="-620" windowWidth="38400" windowHeight="21100" xr2:uid="{07068760-EA20-DB4D-BBEF-E64F73D6D957}"/>
+    <workbookView xWindow="38700" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{07068760-EA20-DB4D-BBEF-E64F73D6D957}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,12 +339,6 @@
     <t>Microchip</t>
   </si>
   <si>
-    <t>QFN-20</t>
-  </si>
-  <si>
-    <t>Single cell, Li-Ion/Li-Po charge management controller</t>
-  </si>
-  <si>
     <t xml:space="preserve">    U2</t>
   </si>
   <si>
@@ -478,6 +472,12 @@
   </si>
   <si>
     <t>SS-52400-003 for standard 1.6 mm PCB thickness</t>
+  </si>
+  <si>
+    <t>Single cell, Li-Ion/Li-Po charge management controller. See https://www.snapeda.com/parts/MCP73871-2CAI/ML/Microchip%20Technology/view-part/?ref=search&amp;t=MCP73871</t>
+  </si>
+  <si>
+    <t>QFN50P400X400X100-21N</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,6 +529,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,10 +559,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1" xr:uid="{3B013FD0-0971-5A4F-BE89-C1629EA6565E}"/>
@@ -898,7 +905,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1132,7 +1139,7 @@
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F10">
         <v>1210</v>
@@ -1152,16 +1159,16 @@
         <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1175,7 +1182,7 @@
         <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E12" t="s">
         <v>48</v>
@@ -1533,197 +1540,197 @@
         <v>100</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>148</v>
-      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G33" t="s">
-        <v>106</v>
+      <c r="F33" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" t="s">
         <v>109</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="G35" t="s">
         <v>110</v>
-      </c>
-      <c r="D35" t="s">
-        <v>110</v>
-      </c>
-      <c r="E35" t="s">
-        <v>111</v>
-      </c>
-      <c r="G35" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" t="s">
         <v>113</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="F36" t="s">
         <v>114</v>
       </c>
-      <c r="D36" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="G36" t="s">
         <v>115</v>
-      </c>
-      <c r="F36" t="s">
-        <v>116</v>
-      </c>
-      <c r="G36" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" t="s">
         <v>118</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="F37" t="s">
         <v>119</v>
       </c>
-      <c r="D37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="G37" t="s">
         <v>120</v>
-      </c>
-      <c r="F37" t="s">
-        <v>121</v>
-      </c>
-      <c r="G37" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" t="s">
         <v>123</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="F38" t="s">
         <v>124</v>
       </c>
-      <c r="D38" t="s">
-        <v>124</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="G38" t="s">
         <v>125</v>
-      </c>
-      <c r="F38" t="s">
-        <v>126</v>
-      </c>
-      <c r="G38" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" t="s">
         <v>128</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="F39" t="s">
         <v>129</v>
       </c>
-      <c r="D39" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="G39" t="s">
         <v>130</v>
-      </c>
-      <c r="F39" t="s">
-        <v>131</v>
-      </c>
-      <c r="G39" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" t="s">
         <v>133</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="F40" t="s">
         <v>134</v>
       </c>
-      <c r="D40" t="s">
-        <v>134</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="G40" t="s">
         <v>135</v>
-      </c>
-      <c r="F40" t="s">
-        <v>136</v>
-      </c>
-      <c r="G40" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>